<commit_message>
Manual Testing notes as on july 3rd
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\012Livetech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA6D1419-BE00-4E1C-80A3-0E47D09268E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC423CB-9578-4371-9270-DE37481709A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BF258B6-0441-47D3-980D-A0CAF612A56D}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>Project Name</t>
   </si>
@@ -104,13 +104,88 @@
   </si>
   <si>
     <t>Screenshots</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001</t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC001</t>
+  </si>
+  <si>
+    <t>To validate login using  valid username and valid password</t>
+  </si>
+  <si>
+    <t>user should have registered and verified email</t>
+  </si>
+  <si>
+    <t>start browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>browser should get started</t>
+  </si>
+  <si>
+    <t>launch app</t>
+  </si>
+  <si>
+    <t>https://adactinhotelapp.com/</t>
+  </si>
+  <si>
+    <t>app should get launched</t>
+  </si>
+  <si>
+    <t>reyaz0806</t>
+  </si>
+  <si>
+    <t>username textbox should accpet the 
+text and display the same</t>
+  </si>
+  <si>
+    <t>enter username in username 
+textbox</t>
+  </si>
+  <si>
+    <t>enter password in password 
+textbox</t>
+  </si>
+  <si>
+    <t>reyaz123</t>
+  </si>
+  <si>
+    <t>password textbox should accept the text
+and display as masked</t>
+  </si>
+  <si>
+    <t>click on button</t>
+  </si>
+  <si>
+    <t>login button should be clickable</t>
+  </si>
+  <si>
+    <t xml:space="preserve">app should  navigate to "Serach Hotel" Page </t>
+  </si>
+  <si>
+    <t>Adactin_Login_TS001_TC002</t>
+  </si>
+  <si>
+    <t>To validate login using  Invalid username and valid password</t>
+  </si>
+  <si>
+    <t>reyaz1212</t>
+  </si>
+  <si>
+    <t>App should give below error 
+"	
+Invalid Login details or Your Password might have expired. Click here to reset your password"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +218,13 @@
       <u/>
       <sz val="20"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -203,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -213,7 +295,19 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -531,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB5A85-1055-4ACD-81B3-2A5F2F033F25}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>
@@ -540,10 +634,10 @@
     <col min="1" max="1" width="42.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="31.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.109375" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="32.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="64.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="26.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="18" style="1" bestFit="1" customWidth="1"/>
@@ -607,13 +701,13 @@
       <c r="D6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="9" t="s">
         <v>16</v>
       </c>
       <c r="H6" s="3" t="s">
@@ -632,39 +726,188 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B7" s="5"/>
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="G8" s="7"/>
+    <row r="7" spans="1:12" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="A7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="8">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="25.8" x14ac:dyDescent="0.45">
+      <c r="E8" s="8">
+        <v>2</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>32</v>
+      </c>
       <c r="L8" s="6"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="B13" s="5"/>
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:12" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="G14" s="7"/>
+    <row r="9" spans="1:12" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="E10" s="8">
+        <v>4</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="E11" s="8">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="H12" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="93.6" x14ac:dyDescent="0.45">
+      <c r="A13" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E13" s="8">
+        <v>1</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G13" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="25.8" x14ac:dyDescent="0.45">
+      <c r="E14" s="8">
+        <v>2</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="E15" s="8">
+        <v>3</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="70.2" x14ac:dyDescent="0.45">
+      <c r="E16" s="8">
+        <v>4</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B17" s="5"/>
       <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.45">
+      <c r="E17" s="8">
+        <v>5</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" ht="117" x14ac:dyDescent="0.45">
       <c r="B18" s="5"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="5"/>
-    </row>
-    <row r="20" spans="2:8" ht="25.8" x14ac:dyDescent="0.5">
-      <c r="G20" s="7"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" ht="25.8" x14ac:dyDescent="0.45">
+      <c r="G20" s="10"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.45">
       <c r="B23" s="5"/>
       <c r="D23" s="5"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G24" s="6"/>
+      <c r="G24" s="11"/>
       <c r="H24" s="5"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.45">
@@ -674,7 +917,7 @@
       <c r="B29" s="5"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G30" s="6"/>
+      <c r="G30" s="11"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.45">
       <c r="H31" s="5"/>
@@ -684,7 +927,7 @@
       <c r="D33" s="5"/>
     </row>
     <row r="34" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G34" s="6"/>
+      <c r="G34" s="11"/>
     </row>
     <row r="36" spans="2:8" x14ac:dyDescent="0.45">
       <c r="H36" s="5"/>
@@ -694,7 +937,7 @@
       <c r="D38" s="5"/>
     </row>
     <row r="39" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G39" s="6"/>
+      <c r="G39" s="11"/>
     </row>
     <row r="41" spans="2:8" x14ac:dyDescent="0.45">
       <c r="H41" s="5"/>
@@ -704,14 +947,19 @@
       <c r="D43" s="5"/>
     </row>
     <row r="44" spans="2:8" x14ac:dyDescent="0.45">
-      <c r="G44" s="6"/>
+      <c r="G44" s="11"/>
     </row>
     <row r="48" spans="2:8" x14ac:dyDescent="0.45">
       <c r="H48" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="G8" r:id="rId1" xr:uid="{518608AD-BE13-43BA-9055-7447392141CA}"/>
+    <hyperlink ref="G14" r:id="rId2" xr:uid="{14307104-89E5-4DAC-B324-47F8ABAC807E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Manual Testing notes as on july 4th
</commit_message>
<xml_diff>
--- a/Test Case Template.xlsx
+++ b/Test Case Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\012Livetech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CC423CB-9578-4371-9270-DE37481709A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E57FFAA-38FC-4F07-AB20-A9583A2BF832}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0BF258B6-0441-47D3-980D-A0CAF612A56D}"/>
   </bookViews>
@@ -625,8 +625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FB5A85-1055-4ACD-81B3-2A5F2F033F25}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="D13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.4" x14ac:dyDescent="0.45"/>

</xml_diff>